<commit_message>
measurements and excel updates
</commit_message>
<xml_diff>
--- a/RDFsim/measurements/measurements.xlsx
+++ b/RDFsim/measurements/measurements.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="moviesGRAPHS" localSheetId="2">Sheet3!$A$2:$D$12</definedName>
     <definedName name="moviesIndexing" localSheetId="0">Sheet1!$A$105:$D$205</definedName>
     <definedName name="moviesIndexing_1" localSheetId="0">Sheet1!$A$3:$D$103</definedName>
     <definedName name="moviesTOPK" localSheetId="1">Sheet2!$A$3:$F$1201</definedName>
@@ -31,7 +33,17 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="moviesIndexing" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" name="moviesGRAPHS" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\tmp\moviesGRAPHS.txt" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="moviesIndexing" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\tmp\moviesIndexing.txt" comma="1" semicolon="1">
       <textFields count="3">
         <textField/>
@@ -40,7 +52,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="moviesIndexing1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" name="moviesIndexing1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\tmp\moviesIndexing.txt" comma="1">
       <textFields count="3">
         <textField/>
@@ -49,7 +61,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="moviesTOPK" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" name="moviesTOPK" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\tmp\moviesTOPK.txt" comma="1">
       <textFields count="4">
         <textField/>
@@ -59,7 +71,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="philosophersIndexing" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="5" name="philosophersIndexing" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\tmp\philosophersIndexing.txt" comma="1">
       <textFields count="3">
         <textField/>
@@ -68,7 +80,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="philosophersTOPK" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="6" name="philosophersTOPK" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\tmp\philosophersTOPK.txt" comma="1">
       <textFields count="4">
         <textField/>
@@ -78,7 +90,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="programmingLangsIndexing" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="7" name="programmingLangsIndexing" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\tmp\programmingLangsIndexing.txt" comma="1">
       <textFields count="3">
         <textField/>
@@ -87,7 +99,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="videoGamesIndexing" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="8" name="videoGamesIndexing" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\tmp\videoGamesIndexing.txt" comma="1">
       <textFields count="3">
         <textField/>
@@ -96,7 +108,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="videoGamesTOPK" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="9" name="videoGamesTOPK" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\tmp\videoGamesTOPK.txt" comma="1">
       <textFields count="4">
         <textField/>
@@ -110,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7672" uniqueCount="2670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7675" uniqueCount="2673">
   <si>
     <t>Movies</t>
   </si>
@@ -8120,6 +8132,15 @@
   </si>
   <si>
     <t>http://dbpedia.org/resource/D/Generation</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/Wedding_Cha_Shinema</t>
+  </si>
+  <si>
+    <t>http://dbpedia.org/resource/The_Morning_After_(1986_film)</t>
+  </si>
+  <si>
+    <t>GRAPHS</t>
   </si>
 </sst>
 </file>
@@ -8159,7 +8180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8184,6 +8205,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -8198,7 +8225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -8207,6 +8234,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8226,35 +8255,39 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="videoGamesIndexing" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="moviesIndexing" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="philosophersIndexing" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="programmingLangsIndexing" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="moviesIndexing_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="videoGamesIndexing" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="moviesIndexing" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="philosophersIndexing" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="programmingLangsIndexing" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="moviesIndexing_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="videoGamesTOPK" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="philosophersTOPK" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="philosophersTOPK" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="moviesTOPK" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="moviesTOPK" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="videoGamesTOPK" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="moviesGRAPHS" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8522,8 +8555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA118"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131:A136"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8531,7 +8564,7 @@
     <col min="1" max="1" width="92.140625" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="59.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -12817,28 +12850,28 @@
       <c r="P108" s="1"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
+      <c r="A109" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="C109" s="4" t="s">
+      <c r="C109" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="E109" s="4" t="s">
+      <c r="E109" s="8" t="s">
         <v>411</v>
       </c>
-      <c r="F109" s="4" t="s">
+      <c r="F109" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="G109" s="4"/>
+      <c r="G109" s="8"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
+      <c r="A110" s="8" t="s">
         <v>104</v>
       </c>
       <c r="B110">
@@ -12855,7 +12888,7 @@
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A111" s="4" t="s">
+      <c r="A111" s="8" t="s">
         <v>306</v>
       </c>
       <c r="B111">
@@ -12872,7 +12905,7 @@
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="8" t="s">
         <v>205</v>
       </c>
       <c r="B112">
@@ -12889,7 +12922,7 @@
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B113">
@@ -12906,14 +12939,14 @@
       </c>
     </row>
     <row r="118" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B118" s="6"/>
-      <c r="C118" s="6"/>
-      <c r="D118" s="6"/>
-      <c r="E118" s="6"/>
-      <c r="F118" s="6"/>
-      <c r="G118" s="6"/>
-      <c r="H118" s="6"/>
-      <c r="I118" s="6"/>
+      <c r="B118" s="9"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9"/>
+      <c r="G118" s="9"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="9"/>
       <c r="J118" s="6"/>
       <c r="K118" s="6"/>
       <c r="L118" s="6"/>
@@ -12936,7 +12969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -54894,4 +54927,169 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2672</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2670</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.06</v>
+      </c>
+      <c r="C3">
+        <v>0.11</v>
+      </c>
+      <c r="D3">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.05</v>
+      </c>
+      <c r="C4">
+        <v>0.45</v>
+      </c>
+      <c r="D4">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0.05</v>
+      </c>
+      <c r="C5">
+        <v>1.29</v>
+      </c>
+      <c r="D5">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>0.03</v>
+      </c>
+      <c r="C6">
+        <v>1.59</v>
+      </c>
+      <c r="D6">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2671</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0.37</v>
+      </c>
+      <c r="C9">
+        <v>0.53</v>
+      </c>
+      <c r="D9">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.39</v>
+      </c>
+      <c r="C10">
+        <v>1.97</v>
+      </c>
+      <c r="D10">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.37</v>
+      </c>
+      <c r="C11">
+        <v>2.6</v>
+      </c>
+      <c r="D11">
+        <v>19.73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0.37</v>
+      </c>
+      <c r="C12">
+        <v>3.42</v>
+      </c>
+      <c r="D12">
+        <v>45.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>